<commit_message>
Some changes in interface
</commit_message>
<xml_diff>
--- a/settings/Settings.xlsx
+++ b/settings/Settings.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlados\forpython\Programm_for_razoom\settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ForPython\Razoom-laser\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10635"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -161,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,6 +188,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -195,6 +206,1087 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Анод. </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>config!$J$4:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>config!$L$4:$L$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C797-4CF1-800D-B324B26DC311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="548729951"/>
+        <c:axId val="548727039"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="548729951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548727039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="548727039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="900"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548729951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>197223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,18 +1554,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +1583,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -499,7 +1591,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -507,24 +1599,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <f>D4*E4</f>
-        <v>1500</v>
-      </c>
-      <c r="G4">
-        <f>F4/$F$1</f>
-        <v>1.8749999999999999E-2</v>
-      </c>
-      <c r="H4">
-        <v>1100</v>
-      </c>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J4">
         <v>0.02</v>
       </c>
@@ -536,26 +1611,9 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F6" si="0">D5*E5</f>
-        <v>5000</v>
-      </c>
-      <c r="G5">
-        <f>F5/$F$1</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="H5">
-        <v>1500</v>
-      </c>
       <c r="J5">
         <v>0.03</v>
       </c>
@@ -564,28 +1622,11 @@
         <v>1250</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L29" si="1">MROUND(K5,100)</f>
+        <f t="shared" ref="L5:L29" si="0">MROUND(K5,100)</f>
         <v>1300</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>200</v>
-      </c>
-      <c r="E6">
-        <v>150</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>30000</v>
-      </c>
-      <c r="G6">
-        <f>F6/$F$1</f>
-        <v>0.375</v>
-      </c>
-      <c r="H6">
-        <v>2000</v>
-      </c>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J6">
         <v>0.04</v>
       </c>
@@ -594,27 +1635,13 @@
         <v>1400</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="D7">
-        <v>170</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <f>E7*D7</f>
-        <v>3400</v>
-      </c>
-      <c r="G7">
-        <f>F7/$F$1</f>
-        <v>4.2500000000000003E-2</v>
-      </c>
       <c r="J7">
         <v>0.06</v>
       </c>
@@ -622,29 +1649,12 @@
         <v>1500</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8">
-        <v>60</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F8:F10" si="2">E8*D8</f>
-        <v>6000</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G8:G10" si="3">F8/$F$1</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H8">
-        <f>MROUND(G8,0.02)</f>
-        <v>0.08</v>
-      </c>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G8" s="6"/>
       <c r="J8">
         <v>0.08</v>
       </c>
@@ -653,454 +1663,458 @@
         <v>1525</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="J9">
         <v>0.1</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" ref="K9:K29" si="4">K8+(100/4)</f>
+        <f t="shared" ref="K9:K29" si="1">K8+(100/4)</f>
         <v>1550</v>
       </c>
       <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <v>200</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10" si="2">E10*D10</f>
+        <v>40000</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10" si="3">F10/$F$1</f>
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <f>MROUND(( 717985*(G10^5) - 1000000*(G10^4) + 544980*(G10^3) - 132653*(G10^2) + 15638*G10 + 901.75),100)</f>
+        <v>3600</v>
+      </c>
+      <c r="J10">
+        <v>0.12</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>1575</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="H11" s="8"/>
+      <c r="J11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K11" s="7">
         <f t="shared" si="1"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0.12</v>
-      </c>
-      <c r="K10" s="7">
-        <f t="shared" si="4"/>
-        <v>1575</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
+      <c r="L11">
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="J11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K11" s="7">
-        <f t="shared" si="4"/>
-        <v>1600</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>0.16</v>
       </c>
       <c r="K12" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1625</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="J13">
         <v>0.18</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1650</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1700</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>0.2</v>
       </c>
       <c r="K14" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1675</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1700</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="J15">
         <v>0.22</v>
       </c>
       <c r="K15" s="7">
-        <f t="shared" si="4"/>
-        <v>1700</v>
-      </c>
-      <c r="L15">
         <f t="shared" si="1"/>
         <v>1700</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J16">
         <v>0.24</v>
       </c>
       <c r="K16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1725</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1700</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="J17">
         <v>0.26</v>
       </c>
       <c r="K17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1750</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1800</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J18">
         <v>0.28000000000000003</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1775</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1800</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="J19">
         <v>0.3</v>
       </c>
       <c r="K19" s="7">
-        <f t="shared" si="4"/>
-        <v>1800</v>
-      </c>
-      <c r="L19">
         <f t="shared" si="1"/>
         <v>1800</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J20">
         <v>0.32</v>
       </c>
       <c r="K20" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1825</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1800</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="J21">
         <v>0.34</v>
       </c>
       <c r="K21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1850</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J22">
         <v>0.36</v>
       </c>
       <c r="K22" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1875</v>
       </c>
       <c r="L22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="J23">
         <v>0.38</v>
       </c>
       <c r="K23" s="7">
-        <f t="shared" si="4"/>
-        <v>1900</v>
-      </c>
-      <c r="L23">
         <f t="shared" si="1"/>
         <v>1900</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J24">
         <v>0.4</v>
       </c>
       <c r="K24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1925</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="J25">
         <v>0.42</v>
       </c>
       <c r="K25" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1950</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J26">
         <v>0.44</v>
       </c>
       <c r="K26" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1975</v>
       </c>
       <c r="L26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="J27">
         <v>0.46</v>
       </c>
       <c r="K27" s="7">
-        <f t="shared" si="4"/>
-        <v>2000</v>
-      </c>
-      <c r="L27">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J28">
         <v>0.48</v>
       </c>
       <c r="K28" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
       <c r="L28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="J29">
         <v>0.5</v>
       </c>
       <c r="K29" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2050</v>
       </c>
       <c r="L29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2100</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L30" s="7"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>